<commit_message>
All pre-database steps done
</commit_message>
<xml_diff>
--- a/bulk_import_tool/IMM import template - test - Copy.xlsx
+++ b/bulk_import_tool/IMM import template - test - Copy.xlsx
@@ -14,7 +14,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="325" uniqueCount="304">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="302" uniqueCount="295">
   <si>
     <t>Catalogue</t>
   </si>
@@ -826,9 +826,6 @@
     <t>Test item 1</t>
   </si>
   <si>
-    <t>Test item 2</t>
-  </si>
-  <si>
     <t>Import test collection</t>
   </si>
   <si>
@@ -862,42 +859,21 @@
     <t>British Columbia</t>
   </si>
   <si>
-    <t>Victoria: RBCM Exhibits building</t>
-  </si>
-  <si>
     <t>Victoria: RBCM Collections building</t>
   </si>
   <si>
     <t>Fannin tower, 2nd floor</t>
   </si>
   <si>
-    <t>Clifford Carl Hall</t>
-  </si>
-  <si>
-    <t>Meg Sugrue, David Stewart</t>
-  </si>
-  <si>
     <t>TEST_CN_01</t>
   </si>
   <si>
-    <t>TEST_CN_02</t>
-  </si>
-  <si>
     <t>FN_01</t>
   </si>
   <si>
-    <t>FN_02</t>
-  </si>
-  <si>
     <t>Cancer productus</t>
   </si>
   <si>
-    <t>Cancer magister</t>
-  </si>
-  <si>
-    <t>Henry Choong; Heidi Gartner</t>
-  </si>
-  <si>
     <t>Ethanol - 70%</t>
   </si>
   <si>
@@ -923,9 +899,6 @@
   </si>
   <si>
     <t>UnitType.unit_cd</t>
-  </si>
-  <si>
-    <t>EV2</t>
   </si>
 </sst>
 </file>
@@ -1370,9 +1343,9 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:EF5"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="C1" workbookViewId="0">
+    <sheetView tabSelected="1" workbookViewId="0">
       <pane ySplit="3" topLeftCell="A4" activePane="bottomLeft" state="frozen"/>
-      <selection pane="bottomLeft" activeCell="W5" sqref="W5"/>
+      <selection pane="bottomLeft" activeCell="A4" sqref="A4"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -2114,7 +2087,7 @@
         <v>110</v>
       </c>
       <c r="AP3" s="11" t="s">
-        <v>299</v>
+        <v>291</v>
       </c>
       <c r="AQ3" s="11" t="s">
         <v>111</v>
@@ -2357,7 +2330,7 @@
         <v>245</v>
       </c>
       <c r="DS3" s="14" t="s">
-        <v>300</v>
+        <v>292</v>
       </c>
       <c r="DT3" s="14" t="s">
         <v>246</v>
@@ -2381,7 +2354,7 @@
         <v>261</v>
       </c>
       <c r="EA3" s="15" t="s">
-        <v>301</v>
+        <v>293</v>
       </c>
       <c r="EB3" s="15" t="s">
         <v>262</v>
@@ -2390,7 +2363,7 @@
         <v>263</v>
       </c>
       <c r="ED3" s="15" t="s">
-        <v>302</v>
+        <v>294</v>
       </c>
       <c r="EE3" s="15" t="s">
         <v>264</v>
@@ -2401,37 +2374,37 @@
     </row>
     <row r="4" spans="1:136" x14ac:dyDescent="0.25">
       <c r="B4" t="s">
-        <v>287</v>
+        <v>283</v>
       </c>
       <c r="C4" t="s">
-        <v>289</v>
+        <v>284</v>
       </c>
       <c r="D4" t="s">
         <v>269</v>
       </c>
       <c r="F4" t="s">
+        <v>270</v>
+      </c>
+      <c r="H4" t="s">
         <v>271</v>
-      </c>
-      <c r="H4" t="s">
-        <v>272</v>
       </c>
       <c r="I4" s="17">
         <v>43465</v>
       </c>
       <c r="K4" t="s">
+        <v>272</v>
+      </c>
+      <c r="M4" t="s">
         <v>273</v>
       </c>
-      <c r="M4" t="s">
+      <c r="N4" t="s">
         <v>274</v>
       </c>
-      <c r="N4" t="s">
+      <c r="Q4" t="s">
         <v>275</v>
       </c>
-      <c r="Q4" t="s">
+      <c r="W4" t="s">
         <v>276</v>
-      </c>
-      <c r="W4" t="s">
-        <v>277</v>
       </c>
       <c r="AE4">
         <v>15</v>
@@ -2440,22 +2413,22 @@
         <v>14</v>
       </c>
       <c r="AH4" t="s">
+        <v>277</v>
+      </c>
+      <c r="AK4" t="s">
+        <v>279</v>
+      </c>
+      <c r="AL4" t="s">
         <v>278</v>
       </c>
-      <c r="AK4" t="s">
+      <c r="AT4" t="s">
         <v>280</v>
       </c>
-      <c r="AL4" t="s">
-        <v>279</v>
-      </c>
-      <c r="AT4" t="s">
+      <c r="AX4" t="s">
+        <v>282</v>
+      </c>
+      <c r="AZ4" t="s">
         <v>281</v>
-      </c>
-      <c r="AX4" t="s">
-        <v>284</v>
-      </c>
-      <c r="AZ4" t="s">
-        <v>283</v>
       </c>
       <c r="BH4">
         <v>48.419603000000002</v>
@@ -2467,121 +2440,33 @@
         <v>43465</v>
       </c>
       <c r="BX4" t="s">
-        <v>291</v>
+        <v>285</v>
       </c>
       <c r="BY4" t="s">
-        <v>277</v>
+        <v>276</v>
       </c>
       <c r="DI4" t="s">
-        <v>296</v>
+        <v>288</v>
       </c>
       <c r="DJ4" t="s">
-        <v>295</v>
+        <v>287</v>
       </c>
       <c r="DM4" t="s">
-        <v>294</v>
+        <v>286</v>
       </c>
       <c r="DT4">
         <v>1</v>
       </c>
       <c r="DV4" t="s">
-        <v>297</v>
+        <v>289</v>
       </c>
       <c r="DW4" t="s">
-        <v>298</v>
+        <v>290</v>
       </c>
     </row>
     <row r="5" spans="1:136" x14ac:dyDescent="0.25">
-      <c r="B5" t="s">
-        <v>288</v>
-      </c>
-      <c r="C5" t="s">
-        <v>290</v>
-      </c>
-      <c r="D5" t="s">
-        <v>270</v>
-      </c>
-      <c r="F5" t="s">
-        <v>271</v>
-      </c>
-      <c r="H5" t="s">
-        <v>272</v>
-      </c>
-      <c r="I5" s="17">
-        <v>43465</v>
-      </c>
-      <c r="K5" t="s">
-        <v>273</v>
-      </c>
-      <c r="M5" t="s">
-        <v>303</v>
-      </c>
-      <c r="N5" t="s">
-        <v>275</v>
-      </c>
-      <c r="Q5" t="s">
-        <v>276</v>
-      </c>
-      <c r="W5" t="s">
-        <v>286</v>
-      </c>
-      <c r="AE5">
-        <v>5</v>
-      </c>
-      <c r="AF5">
-        <v>4</v>
-      </c>
-      <c r="AH5" t="s">
-        <v>278</v>
-      </c>
-      <c r="AK5" t="s">
-        <v>280</v>
-      </c>
-      <c r="AL5" t="s">
-        <v>279</v>
-      </c>
-      <c r="AT5" t="s">
-        <v>281</v>
-      </c>
-      <c r="AX5" t="s">
-        <v>285</v>
-      </c>
-      <c r="AZ5" t="s">
-        <v>282</v>
-      </c>
-      <c r="BH5">
-        <v>48.419956999999997</v>
-      </c>
-      <c r="BJ5">
-        <v>-123.3688604</v>
-      </c>
-      <c r="BV5" s="17">
-        <v>43465</v>
-      </c>
-      <c r="BX5" t="s">
-        <v>292</v>
-      </c>
-      <c r="BY5" t="s">
-        <v>293</v>
-      </c>
-      <c r="DI5" t="s">
-        <v>296</v>
-      </c>
-      <c r="DJ5" t="s">
-        <v>295</v>
-      </c>
-      <c r="DM5" t="s">
-        <v>294</v>
-      </c>
-      <c r="DT5">
-        <v>1</v>
-      </c>
-      <c r="DV5" t="s">
-        <v>297</v>
-      </c>
-      <c r="DW5" t="s">
-        <v>298</v>
-      </c>
+      <c r="I5" s="17"/>
+      <c r="BV5" s="17"/>
     </row>
   </sheetData>
   <mergeCells count="7">

</xml_diff>